<commit_message>
Deleting accidental extra gantt chart
</commit_message>
<xml_diff>
--- a/Team_Gantt_Chart.xlsx
+++ b/Team_Gantt_Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Brandon Foss\Documents\GitHub\6_Angry_Devs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08871F43-CEB5-4FF5-B76F-AE3281895761}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47EEDD6E-CEB5-436E-A5FA-54089FB0346A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12030" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Management Summary" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="78">
   <si>
     <t>testing</t>
   </si>
@@ -1173,8 +1173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:Q10"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1537,11 +1537,11 @@
       </c>
       <c r="D9" s="41">
         <f t="shared" si="7"/>
-        <v>950</v>
+        <v>750</v>
       </c>
       <c r="E9" s="27">
         <f t="shared" si="8"/>
-        <v>3950</v>
+        <v>4150</v>
       </c>
       <c r="G9" s="14">
         <f>(Gantt!$B52)*100</f>
@@ -1560,11 +1560,11 @@
       </c>
       <c r="L9" s="15">
         <f>Meetings!B9*100</f>
-        <v>550</v>
+        <v>350</v>
       </c>
       <c r="M9" s="16">
         <f t="shared" si="10"/>
-        <v>1950</v>
+        <v>2150</v>
       </c>
       <c r="O9" s="54">
         <f>(SA!C32)*100</f>
@@ -1589,11 +1589,11 @@
       </c>
       <c r="D10" s="25">
         <f>SUM(D4:D9)</f>
-        <v>10850</v>
+        <v>10650</v>
       </c>
       <c r="E10" s="26">
         <f>SUM(E4:E9)</f>
-        <v>30450</v>
+        <v>30650</v>
       </c>
       <c r="G10" s="17">
         <f>SUM(G4:G9)</f>
@@ -1613,11 +1613,11 @@
       </c>
       <c r="L10" s="18">
         <f>SUM(L4:L9)</f>
-        <v>4150</v>
+        <v>3950</v>
       </c>
       <c r="M10" s="19">
         <f>SUM(M4:M9)</f>
-        <v>10850</v>
+        <v>11050</v>
       </c>
       <c r="O10" s="24">
         <f>SUM(O4:O9)</f>
@@ -1648,7 +1648,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AF66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -4141,7 +4141,7 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4397,7 +4397,7 @@
       </c>
       <c r="B9" s="72">
         <f t="shared" si="0"/>
-        <v>5.5</v>
+        <v>3.5</v>
       </c>
       <c r="C9" s="71" t="s">
         <v>12</v>
@@ -4406,9 +4406,7 @@
         <v>12</v>
       </c>
       <c r="E9" s="68"/>
-      <c r="F9" s="73" t="s">
-        <v>12</v>
-      </c>
+      <c r="F9" s="73"/>
       <c r="G9" s="73"/>
       <c r="H9" s="74"/>
       <c r="I9" s="74"/>
@@ -4422,7 +4420,7 @@
       </c>
       <c r="B10" s="64">
         <f>SUM(B4:B9)</f>
-        <v>41.5</v>
+        <v>39.5</v>
       </c>
       <c r="C10" s="64">
         <f>COUNTIF(C4:C9,"*ü*") * C3</f>
@@ -4438,7 +4436,7 @@
       </c>
       <c r="F10" s="64">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G10" s="64">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
Updated gantt chart for meeting
</commit_message>
<xml_diff>
--- a/Team_Gantt_Chart.xlsx
+++ b/Team_Gantt_Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Brandon Foss\Documents\GitHub\6_Angry_Devs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47EEDD6E-CEB5-436E-A5FA-54089FB0346A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08209D89-A7A0-4441-8738-0606AD17FF64}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12030" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Management Summary" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="79">
   <si>
     <t>testing</t>
   </si>
@@ -267,6 +267,9 @@
   </si>
   <si>
     <t>track time changes</t>
+  </si>
+  <si>
+    <t>Initial Demo Prep / Game start</t>
   </si>
 </sst>
 </file>
@@ -1173,7 +1176,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:Q10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
@@ -1269,11 +1272,11 @@
       </c>
       <c r="D4" s="21">
         <f t="shared" ref="D4:D7" si="0">(H4+L4 +P4)</f>
-        <v>2350</v>
+        <v>2550</v>
       </c>
       <c r="E4" s="22">
         <f>(C4-D4)</f>
-        <v>4150</v>
+        <v>3950</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="14">
@@ -1293,11 +1296,11 @@
       </c>
       <c r="L4" s="21">
         <f>Meetings!B4*100</f>
-        <v>750</v>
+        <v>950</v>
       </c>
       <c r="M4" s="22">
         <f>(K4-L4)</f>
-        <v>1750</v>
+        <v>1550</v>
       </c>
       <c r="O4" s="47">
         <f>(SA!C7)*100</f>
@@ -1322,11 +1325,11 @@
       </c>
       <c r="D5" s="15">
         <f t="shared" si="0"/>
-        <v>1950</v>
+        <v>2150</v>
       </c>
       <c r="E5" s="16">
         <f t="shared" ref="E5:E7" si="2">(C5-D5)</f>
-        <v>10050</v>
+        <v>9850</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="14">
@@ -1346,11 +1349,11 @@
       </c>
       <c r="L5" s="15">
         <f>Meetings!B5*100</f>
-        <v>750</v>
+        <v>950</v>
       </c>
       <c r="M5" s="16">
         <f t="shared" ref="M5:M7" si="4">(K5-L5)</f>
-        <v>1750</v>
+        <v>1550</v>
       </c>
       <c r="O5" s="44">
         <f>(SA!C12)*100</f>
@@ -1429,11 +1432,11 @@
       </c>
       <c r="D7" s="45">
         <f t="shared" si="0"/>
-        <v>1700</v>
+        <v>1900</v>
       </c>
       <c r="E7" s="46">
         <f t="shared" si="2"/>
-        <v>4200</v>
+        <v>4000</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="14">
@@ -1453,11 +1456,11 @@
       </c>
       <c r="L7" s="15">
         <f>Meetings!B7*100</f>
-        <v>600</v>
+        <v>800</v>
       </c>
       <c r="M7" s="16">
         <f t="shared" si="4"/>
-        <v>1900</v>
+        <v>1700</v>
       </c>
       <c r="N7" s="42"/>
       <c r="O7" s="56">
@@ -1589,11 +1592,11 @@
       </c>
       <c r="D10" s="25">
         <f>SUM(D4:D9)</f>
-        <v>10650</v>
+        <v>11250</v>
       </c>
       <c r="E10" s="26">
         <f>SUM(E4:E9)</f>
-        <v>30650</v>
+        <v>30050</v>
       </c>
       <c r="G10" s="17">
         <f>SUM(G4:G9)</f>
@@ -1613,11 +1616,11 @@
       </c>
       <c r="L10" s="18">
         <f>SUM(L4:L9)</f>
-        <v>3950</v>
+        <v>4550</v>
       </c>
       <c r="M10" s="19">
         <f>SUM(M4:M9)</f>
-        <v>11050</v>
+        <v>10450</v>
       </c>
       <c r="O10" s="24">
         <f>SUM(O4:O9)</f>
@@ -1648,7 +1651,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AF66"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -4141,13 +4144,14 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="13.140625" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -4204,7 +4208,7 @@
         <v>75</v>
       </c>
       <c r="G2" s="67" t="s">
-        <v>39</v>
+        <v>78</v>
       </c>
       <c r="H2" s="67" t="s">
         <v>39</v>
@@ -4240,7 +4244,7 @@
         <v>2</v>
       </c>
       <c r="G3" s="66">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H3" s="66">
         <v>0</v>
@@ -4264,7 +4268,7 @@
       </c>
       <c r="B4" s="70">
         <f t="shared" ref="B4:B9" si="0">SUMIF(C4:L4,A$12,C$3:Z$3)</f>
-        <v>7.5</v>
+        <v>9.5</v>
       </c>
       <c r="C4" s="68" t="s">
         <v>12</v>
@@ -4278,7 +4282,9 @@
       <c r="F4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="68"/>
+      <c r="G4" s="68" t="s">
+        <v>12</v>
+      </c>
       <c r="H4" s="69"/>
       <c r="I4" s="69"/>
       <c r="J4" s="68"/>
@@ -4291,7 +4297,7 @@
       </c>
       <c r="B5" s="70">
         <f t="shared" si="0"/>
-        <v>7.5</v>
+        <v>9.5</v>
       </c>
       <c r="C5" s="68" t="s">
         <v>12</v>
@@ -4305,7 +4311,9 @@
       <c r="F5" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="68"/>
+      <c r="G5" s="68" t="s">
+        <v>12</v>
+      </c>
       <c r="H5" s="69"/>
       <c r="I5" s="69"/>
       <c r="J5" s="68"/>
@@ -4345,7 +4353,7 @@
       </c>
       <c r="B7" s="70">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C7" s="68"/>
       <c r="D7" s="68" t="s">
@@ -4357,7 +4365,9 @@
       <c r="F7" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="68"/>
+      <c r="G7" s="68" t="s">
+        <v>12</v>
+      </c>
       <c r="H7" s="69"/>
       <c r="I7" s="69"/>
       <c r="J7" s="68"/>
@@ -4420,7 +4430,7 @@
       </c>
       <c r="B10" s="64">
         <f>SUM(B4:B9)</f>
-        <v>39.5</v>
+        <v>45.5</v>
       </c>
       <c r="C10" s="64">
         <f>COUNTIF(C4:C9,"*ü*") * C3</f>
@@ -4440,7 +4450,7 @@
       </c>
       <c r="G10" s="64">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H10" s="64">
         <f t="shared" si="1"/>

</xml_diff>